<commit_message>
Default var series + leontief method for EOP
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/techdata_adv.xlsx
+++ b/examples/Abatement/Data/techdata_adv.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="inputdisp" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>unit_cost</t>
   </si>
@@ -50,12 +50,6 @@
     <t>CO2_overlap_2_othertechs</t>
   </si>
   <si>
-    <t>CO2_overlap_3_potshare</t>
-  </si>
-  <si>
-    <t>CO2_overlap_3_othertechs</t>
-  </si>
-  <si>
     <t>EL_coverage_pot</t>
   </si>
   <si>
@@ -180,6 +174,24 @@
   </si>
   <si>
     <t>input_share_coal</t>
+  </si>
+  <si>
+    <t>NOX_coverage_pot</t>
+  </si>
+  <si>
+    <t>NOX_coverage_curr</t>
+  </si>
+  <si>
+    <t>NOX_overlap_1_potshare</t>
+  </si>
+  <si>
+    <t>NOX_overlap_1_othertechs</t>
+  </si>
+  <si>
+    <t>NOX_overlap_2_potshare</t>
+  </si>
+  <si>
+    <t>NOX_overlap_2_othertechs</t>
   </si>
 </sst>
 </file>
@@ -500,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="K14" sqref="K14"/>
     </sheetView>
@@ -517,37 +529,37 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
         <v>32</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" t="s">
-        <v>34</v>
       </c>
       <c r="L1" t="s">
         <v>0</v>
@@ -565,33 +577,33 @@
         <v>4</v>
       </c>
       <c r="Q1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="W1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -609,18 +621,18 @@
         <v>0.5</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O2">
         <v>0.4</v>
       </c>
       <c r="P2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -638,18 +650,18 @@
         <v>0.25</v>
       </c>
       <c r="R3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S3">
         <v>0.3</v>
       </c>
       <c r="T3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -666,7 +678,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -684,18 +696,18 @@
         <v>0.25</v>
       </c>
       <c r="V5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="W5">
         <v>0.5</v>
       </c>
       <c r="X5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -716,12 +728,12 @@
         <v>0.25</v>
       </c>
       <c r="N6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -742,12 +754,12 @@
         <v>0.1</v>
       </c>
       <c r="N7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -768,12 +780,12 @@
         <v>0.1</v>
       </c>
       <c r="R8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -797,12 +809,12 @@
         <v>0.125</v>
       </c>
       <c r="R9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -823,12 +835,12 @@
         <v>6.25E-2</v>
       </c>
       <c r="V10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -849,7 +861,7 @@
         <v>0.1</v>
       </c>
       <c r="X11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -859,69 +871,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E4" sqref="E4"/>
+      <selection pane="topRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="17" customWidth="1"/>
-    <col min="6" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="14" width="23.7109375" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="1" max="7" width="17" customWidth="1"/>
+    <col min="8" max="9" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="18" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
       <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>52</v>
       </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
       <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
         <v>0</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -935,19 +958,25 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>0.3</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0.01</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>0.2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -961,14 +990,66 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>0.3</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>0.02</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>6.5</v>
+      </c>
+      <c r="K3">
+        <v>0.2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0.3</v>
+      </c>
+      <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="O4">
+        <v>0.5</v>
+      </c>
+      <c r="P4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+      <c r="G5">
+        <v>0.02</v>
+      </c>
+      <c r="J5">
+        <v>11</v>
+      </c>
+      <c r="O5">
+        <v>0.5</v>
+      </c>
+      <c r="P5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -991,15 +1072,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1007,7 +1088,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1015,7 +1096,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1023,7 +1104,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1031,7 +1112,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>1</v>

</xml_diff>

<commit_message>
scale-parametre indført. kan ikke køre lige pt
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/techdata_adv.xlsx
+++ b/examples/Abatement/Data/techdata_adv.xlsx
@@ -875,7 +875,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I6" sqref="I6"/>
+      <selection pane="topRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1017,7 @@
         <v>0.3</v>
       </c>
       <c r="G4">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="J4">
         <v>7</v>
@@ -1040,7 +1040,7 @@
         <v>0.3</v>
       </c>
       <c r="G5">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="J5">
         <v>11</v>

</xml_diff>